<commit_message>
updated udid which was missed
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA0DEC-23D9-A247-A674-B1FC23FB8CA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{108CD4CB-519C-4248-A071-FE764E3909BF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1260" windowWidth="28040" windowHeight="16500" activeTab="2" xr2:uid="{F5AD2FE8-A01F-1E49-94AB-A1FBFAACC706}"/>
+    <workbookView activeTab="1" windowHeight="16500" windowWidth="28040" xWindow="20" xr2:uid="{F5AD2FE8-A01F-1E49-94AB-A1FBFAACC706}" yWindow="540"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" sheetId="1" r:id="rId1"/>
-    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
-    <sheet name="config_automation_phone" sheetId="3" r:id="rId3"/>
-    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId4"/>
-    <sheet name="config_fsa_track_build" sheetId="5" r:id="rId5"/>
+    <sheet name="config_local" r:id="rId1" sheetId="1"/>
+    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
+    <sheet name="config_automation_phone" r:id="rId3" sheetId="3"/>
+    <sheet name="config_fsa_pqt_build" r:id="rId4" sheetId="4"/>
+    <sheet name="config_fsa_track_build" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="96">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -383,6 +383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -449,29 +450,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -488,10 +489,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -526,7 +527,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -578,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -689,21 +690,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -720,7 +721,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -772,14 +773,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747902-0905-9A4B-A648-FC506DD60323}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747902-0905-9A4B-A648-FC506DD60323}">
   <dimension ref="A1:AN34"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -788,39 +789,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="67" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="52.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="115.33203125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="49" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="74.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="65.83203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="84.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="74.33203125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -915,7 +916,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1138,66 +1139,66 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{65290685-B75F-2F47-A5A2-C5F98F0468A7}"/>
-    <hyperlink ref="R2" r:id="rId2" xr:uid="{A8C94B01-4AE8-4A46-A8C0-F0B6766D6C5A}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{9021A63E-45E4-2247-B495-773BCC48D6BC}"/>
-    <hyperlink ref="T2" r:id="rId4" xr:uid="{111D145D-7C58-0241-B4B7-EC3C95D38325}"/>
-    <hyperlink ref="U2" r:id="rId5" xr:uid="{DA34061A-CC99-BD49-AFD7-59CA373B6607}"/>
-    <hyperlink ref="V2" r:id="rId6" xr:uid="{E3E98677-132E-E64D-A508-185D4810255C}"/>
-    <hyperlink ref="W2" r:id="rId7" xr:uid="{8DB1D18B-EA97-AA4D-9AC7-02A48CDE67A6}"/>
-    <hyperlink ref="X2" r:id="rId8" xr:uid="{64F0B1C6-CD58-A845-A599-DFE23DA422CC}"/>
-    <hyperlink ref="Y2" r:id="rId9" xr:uid="{4FAFCCA4-4F24-0B49-934E-AC441897C9C5}"/>
-    <hyperlink ref="AB2" r:id="rId10" xr:uid="{486C7ACD-3F79-B144-8138-AEDF137735C6}"/>
+    <hyperlink r:id="rId1" ref="P2" xr:uid="{65290685-B75F-2F47-A5A2-C5F98F0468A7}"/>
+    <hyperlink r:id="rId2" ref="R2" xr:uid="{A8C94B01-4AE8-4A46-A8C0-F0B6766D6C5A}"/>
+    <hyperlink r:id="rId3" ref="N2" xr:uid="{9021A63E-45E4-2247-B495-773BCC48D6BC}"/>
+    <hyperlink r:id="rId4" ref="T2" xr:uid="{111D145D-7C58-0241-B4B7-EC3C95D38325}"/>
+    <hyperlink r:id="rId5" ref="U2" xr:uid="{DA34061A-CC99-BD49-AFD7-59CA373B6607}"/>
+    <hyperlink r:id="rId6" ref="V2" xr:uid="{E3E98677-132E-E64D-A508-185D4810255C}"/>
+    <hyperlink r:id="rId7" ref="W2" xr:uid="{8DB1D18B-EA97-AA4D-9AC7-02A48CDE67A6}"/>
+    <hyperlink r:id="rId8" ref="X2" xr:uid="{64F0B1C6-CD58-A845-A599-DFE23DA422CC}"/>
+    <hyperlink r:id="rId9" ref="Y2" xr:uid="{4FAFCCA4-4F24-0B49-934E-AC441897C9C5}"/>
+    <hyperlink r:id="rId10" ref="AB2" xr:uid="{486C7ACD-3F79-B144-8138-AEDF137735C6}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BF172F-CE08-6840-ACF9-880AB6E40DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BF172F-CE08-6840-ACF9-880AB6E40DE2}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1217,13 +1218,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>24</v>
@@ -1295,7 +1296,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1315,13 +1316,13 @@
         <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J2" t="s">
         <v>92</v>
@@ -1395,61 +1396,62 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{2373DCCF-7CF7-6D48-9391-B2017EA3F6CB}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{45EF8F3D-534D-2F45-94E3-C73D8504CC2F}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{317C8481-D29E-9841-A568-E5293BF078E6}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{2250E180-CC76-0844-A14E-BECC396552E1}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{3B6377D4-E37D-8E4E-A566-7D3CA80B53F6}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{08609375-5C82-1140-80FE-D1DE3470E1BE}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{195848E9-E895-054F-8CD9-4B349763F02C}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{2373DCCF-7CF7-6D48-9391-B2017EA3F6CB}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{45EF8F3D-534D-2F45-94E3-C73D8504CC2F}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{317C8481-D29E-9841-A568-E5293BF078E6}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{2250E180-CC76-0844-A14E-BECC396552E1}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{3B6377D4-E37D-8E4E-A566-7D3CA80B53F6}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{08609375-5C82-1140-80FE-D1DE3470E1BE}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{195848E9-E895-054F-8CD9-4B349763F02C}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABD5772-2955-6C46-88A2-787F9D38DC97}">
-  <dimension ref="A1:AE2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABD5772-2955-6C46-88A2-787F9D38DC97}">
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="28" max="30" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="29" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1469,82 +1471,85 @@
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1564,137 +1569,140 @@
         <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{FF8A98B7-8501-6F47-A2FB-10824115B353}"/>
-    <hyperlink ref="T2" r:id="rId2" xr:uid="{E5504FE2-E34C-AD4E-9FED-91F77342117E}"/>
-    <hyperlink ref="U2" r:id="rId3" xr:uid="{E3CFACEB-C525-FB4B-816E-5C98177D7B3A}"/>
-    <hyperlink ref="V2" r:id="rId4" xr:uid="{037F7191-EF8F-1B41-A957-BC232B559744}"/>
-    <hyperlink ref="W2" r:id="rId5" xr:uid="{C6F51406-8912-3748-8B88-9B0A0A8B059D}"/>
-    <hyperlink ref="X2" r:id="rId6" xr:uid="{CDB08067-96F2-2742-872D-1B028C2950EE}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{FF8A98B7-8501-6F47-A2FB-10824115B353}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{E5504FE2-E34C-AD4E-9FED-91F77342117E}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{E3CFACEB-C525-FB4B-816E-5C98177D7B3A}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{037F7191-EF8F-1B41-A957-BC232B559744}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{C6F51406-8912-3748-8B88-9B0A0A8B059D}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{CDB08067-96F2-2742-872D-1B028C2950EE}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACBC21-67F9-9748-8578-54FDD50767ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACBC21-67F9-9748-8578-54FDD50767ED}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="31" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="29" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1892,20 +1900,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{A71DD4B7-4F78-624F-8526-BC2C8DAF91F2}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{1B540CF2-7A50-6B48-8B71-0C274B92DD51}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{91AEDBB0-8784-C240-9F57-F0191D9A7F37}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{4CBB3277-EAC2-1C4C-B5B0-6055F81AEB79}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{43033950-1900-2048-9098-30C4C6B77A36}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{AF882D86-8162-1A40-9D4C-2B7AFACABB92}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{F85A03DD-44E5-6E49-B503-8C6C4E7ECC22}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{A71DD4B7-4F78-624F-8526-BC2C8DAF91F2}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{1B540CF2-7A50-6B48-8B71-0C274B92DD51}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{91AEDBB0-8784-C240-9F57-F0191D9A7F37}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{4CBB3277-EAC2-1C4C-B5B0-6055F81AEB79}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{43033950-1900-2048-9098-30C4C6B77A36}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{AF882D86-8162-1A40-9D4C-2B7AFACABB92}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{F85A03DD-44E5-6E49-B503-8C6C4E7ECC22}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70778CC3-4254-DD46-A825-6190F74A8C8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70778CC3-4254-DD46-A825-6190F74A8C8D}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1914,7 +1922,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2012,7 +2020,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2112,14 +2120,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{B41713CD-0C7A-A94A-9E0C-2C92C9129EB5}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{F8ED6A05-BFC1-7E48-A376-F7EF824AE76F}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{B2E95E89-7408-7140-82FB-6817D1D4C34A}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{7BA77DFF-CF38-3F44-95C3-4775F3663E98}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{A95FE44D-A1CF-E248-A845-0A3B8C68FB3D}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{DCB51B4E-919D-6847-9170-E731E9B9D69D}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{2489425F-B372-874E-8A85-A3A1E07348EE}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{B41713CD-0C7A-A94A-9E0C-2C92C9129EB5}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{F8ED6A05-BFC1-7E48-A376-F7EF824AE76F}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{B2E95E89-7408-7140-82FB-6817D1D4C34A}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{7BA77DFF-CF38-3F44-95C3-4775F3663E98}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{A95FE44D-A1CF-E248-A845-0A3B8C68FB3D}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{DCB51B4E-919D-6847-9170-E731E9B9D69D}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{2489425F-B372-874E-8A85-A3A1E07348EE}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support for browser
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DF8B0C-87A2-E940-A4E6-BB35D8570511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7BCC110B-EF0A-1540-AC45-1CE8C4CDA36D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="540" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{F5AD2FE8-A01F-1E49-94AB-A1FBFAACC706}"/>
+    <workbookView activeTab="1" windowHeight="16500" windowWidth="28040" xWindow="20" xr2:uid="{F5AD2FE8-A01F-1E49-94AB-A1FBFAACC706}" yWindow="540"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" sheetId="1" r:id="rId1"/>
-    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
-    <sheet name="config_automation_phone" sheetId="3" r:id="rId3"/>
-    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId4"/>
-    <sheet name="config_fsa_track_build" sheetId="5" r:id="rId5"/>
+    <sheet name="config_local" r:id="rId1" sheetId="1"/>
+    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
+    <sheet name="config_automation_phone" r:id="rId3" sheetId="3"/>
+    <sheet name="config_fsa_pqt_build" r:id="rId4" sheetId="4"/>
+    <sheet name="config_fsa_track_build" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="98">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -378,11 +378,18 @@
   <si>
     <t>iPhone Developer: Rajesh Rao (76X824PR66)</t>
   </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -449,29 +456,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -488,10 +495,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -526,7 +533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -578,7 +585,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -689,21 +696,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -720,7 +727,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -772,14 +779,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747902-0905-9A4B-A648-FC506DD60323}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747902-0905-9A4B-A648-FC506DD60323}">
   <dimension ref="A1:AN34"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -788,39 +795,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="67" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="52.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="115.33203125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="49" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="74.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="65.83203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="84.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="74.33203125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -915,7 +922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1138,66 +1145,66 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{65290685-B75F-2F47-A5A2-C5F98F0468A7}"/>
-    <hyperlink ref="R2" r:id="rId2" xr:uid="{A8C94B01-4AE8-4A46-A8C0-F0B6766D6C5A}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{9021A63E-45E4-2247-B495-773BCC48D6BC}"/>
-    <hyperlink ref="T2" r:id="rId4" xr:uid="{111D145D-7C58-0241-B4B7-EC3C95D38325}"/>
-    <hyperlink ref="U2" r:id="rId5" xr:uid="{DA34061A-CC99-BD49-AFD7-59CA373B6607}"/>
-    <hyperlink ref="V2" r:id="rId6" xr:uid="{E3E98677-132E-E64D-A508-185D4810255C}"/>
-    <hyperlink ref="W2" r:id="rId7" xr:uid="{8DB1D18B-EA97-AA4D-9AC7-02A48CDE67A6}"/>
-    <hyperlink ref="X2" r:id="rId8" xr:uid="{64F0B1C6-CD58-A845-A599-DFE23DA422CC}"/>
-    <hyperlink ref="Y2" r:id="rId9" xr:uid="{4FAFCCA4-4F24-0B49-934E-AC441897C9C5}"/>
-    <hyperlink ref="AB2" r:id="rId10" xr:uid="{486C7ACD-3F79-B144-8138-AEDF137735C6}"/>
+    <hyperlink r:id="rId1" ref="P2" xr:uid="{65290685-B75F-2F47-A5A2-C5F98F0468A7}"/>
+    <hyperlink r:id="rId2" ref="R2" xr:uid="{A8C94B01-4AE8-4A46-A8C0-F0B6766D6C5A}"/>
+    <hyperlink r:id="rId3" ref="N2" xr:uid="{9021A63E-45E4-2247-B495-773BCC48D6BC}"/>
+    <hyperlink r:id="rId4" ref="T2" xr:uid="{111D145D-7C58-0241-B4B7-EC3C95D38325}"/>
+    <hyperlink r:id="rId5" ref="U2" xr:uid="{DA34061A-CC99-BD49-AFD7-59CA373B6607}"/>
+    <hyperlink r:id="rId6" ref="V2" xr:uid="{E3E98677-132E-E64D-A508-185D4810255C}"/>
+    <hyperlink r:id="rId7" ref="W2" xr:uid="{8DB1D18B-EA97-AA4D-9AC7-02A48CDE67A6}"/>
+    <hyperlink r:id="rId8" ref="X2" xr:uid="{64F0B1C6-CD58-A845-A599-DFE23DA422CC}"/>
+    <hyperlink r:id="rId9" ref="Y2" xr:uid="{4FAFCCA4-4F24-0B49-934E-AC441897C9C5}"/>
+    <hyperlink r:id="rId10" ref="AB2" xr:uid="{486C7ACD-3F79-B144-8138-AEDF137735C6}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BF172F-CE08-6840-ACF9-880AB6E40DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BF172F-CE08-6840-ACF9-880AB6E40DE2}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1295,9 +1302,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>93</v>
@@ -1395,21 +1402,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{2373DCCF-7CF7-6D48-9391-B2017EA3F6CB}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{45EF8F3D-534D-2F45-94E3-C73D8504CC2F}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{317C8481-D29E-9841-A568-E5293BF078E6}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{2250E180-CC76-0844-A14E-BECC396552E1}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{3B6377D4-E37D-8E4E-A566-7D3CA80B53F6}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{08609375-5C82-1140-80FE-D1DE3470E1BE}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{195848E9-E895-054F-8CD9-4B349763F02C}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{2373DCCF-7CF7-6D48-9391-B2017EA3F6CB}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{45EF8F3D-534D-2F45-94E3-C73D8504CC2F}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{317C8481-D29E-9841-A568-E5293BF078E6}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{2250E180-CC76-0844-A14E-BECC396552E1}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{3B6377D4-E37D-8E4E-A566-7D3CA80B53F6}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{08609375-5C82-1140-80FE-D1DE3470E1BE}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{195848E9-E895-054F-8CD9-4B349763F02C}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABD5772-2955-6C46-88A2-787F9D38DC97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABD5772-2955-6C46-88A2-787F9D38DC97}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1418,39 +1425,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="29" max="31" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="29" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1548,7 +1555,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1648,19 +1655,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{FF8A98B7-8501-6F47-A2FB-10824115B353}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{E5504FE2-E34C-AD4E-9FED-91F77342117E}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{E3CFACEB-C525-FB4B-816E-5C98177D7B3A}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{037F7191-EF8F-1B41-A957-BC232B559744}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{C6F51406-8912-3748-8B88-9B0A0A8B059D}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{CDB08067-96F2-2742-872D-1B028C2950EE}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{FF8A98B7-8501-6F47-A2FB-10824115B353}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{E5504FE2-E34C-AD4E-9FED-91F77342117E}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{E3CFACEB-C525-FB4B-816E-5C98177D7B3A}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{037F7191-EF8F-1B41-A957-BC232B559744}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{C6F51406-8912-3748-8B88-9B0A0A8B059D}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{CDB08067-96F2-2742-872D-1B028C2950EE}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACBC21-67F9-9748-8578-54FDD50767ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACBC21-67F9-9748-8578-54FDD50767ED}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1669,39 +1676,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="31" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="29" max="31" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1799,7 +1806,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1899,20 +1906,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{A71DD4B7-4F78-624F-8526-BC2C8DAF91F2}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{1B540CF2-7A50-6B48-8B71-0C274B92DD51}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{91AEDBB0-8784-C240-9F57-F0191D9A7F37}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{4CBB3277-EAC2-1C4C-B5B0-6055F81AEB79}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{43033950-1900-2048-9098-30C4C6B77A36}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{AF882D86-8162-1A40-9D4C-2B7AFACABB92}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{F85A03DD-44E5-6E49-B503-8C6C4E7ECC22}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{A71DD4B7-4F78-624F-8526-BC2C8DAF91F2}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{1B540CF2-7A50-6B48-8B71-0C274B92DD51}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{91AEDBB0-8784-C240-9F57-F0191D9A7F37}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{4CBB3277-EAC2-1C4C-B5B0-6055F81AEB79}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{43033950-1900-2048-9098-30C4C6B77A36}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{AF882D86-8162-1A40-9D4C-2B7AFACABB92}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{F85A03DD-44E5-6E49-B503-8C6C4E7ECC22}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70778CC3-4254-DD46-A825-6190F74A8C8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70778CC3-4254-DD46-A825-6190F74A8C8D}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1921,7 +1928,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2019,7 +2026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2119,14 +2126,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{B41713CD-0C7A-A94A-9E0C-2C92C9129EB5}"/>
-    <hyperlink ref="U2" r:id="rId2" xr:uid="{F8ED6A05-BFC1-7E48-A376-F7EF824AE76F}"/>
-    <hyperlink ref="V2" r:id="rId3" xr:uid="{B2E95E89-7408-7140-82FB-6817D1D4C34A}"/>
-    <hyperlink ref="W2" r:id="rId4" xr:uid="{7BA77DFF-CF38-3F44-95C3-4775F3663E98}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{A95FE44D-A1CF-E248-A845-0A3B8C68FB3D}"/>
-    <hyperlink ref="Y2" r:id="rId6" xr:uid="{DCB51B4E-919D-6847-9170-E731E9B9D69D}"/>
-    <hyperlink ref="AB2" r:id="rId7" xr:uid="{2489425F-B372-874E-8A85-A3A1E07348EE}"/>
+    <hyperlink r:id="rId1" ref="T2" xr:uid="{B41713CD-0C7A-A94A-9E0C-2C92C9129EB5}"/>
+    <hyperlink r:id="rId2" ref="U2" xr:uid="{F8ED6A05-BFC1-7E48-A376-F7EF824AE76F}"/>
+    <hyperlink r:id="rId3" ref="V2" xr:uid="{B2E95E89-7408-7140-82FB-6817D1D4C34A}"/>
+    <hyperlink r:id="rId4" ref="W2" xr:uid="{7BA77DFF-CF38-3F44-95C3-4775F3663E98}"/>
+    <hyperlink r:id="rId5" ref="X2" xr:uid="{A95FE44D-A1CF-E248-A845-0A3B8C68FB3D}"/>
+    <hyperlink r:id="rId6" ref="Y2" xr:uid="{DCB51B4E-919D-6847-9170-E731E9B9D69D}"/>
+    <hyperlink r:id="rId7" ref="AB2" xr:uid="{2489425F-B372-874E-8A85-A3A1E07348EE}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changing the cong file to build org
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3205CCC6-6A4C-AA41-980E-FE84701C1BDB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView windowHeight="16500" windowWidth="28040" xWindow="20" xr2:uid="{F5AD2FE8-A01F-1E49-94AB-A1FBFAACC706}" yWindow="440"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" r:id="rId1" sheetId="1"/>
-    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
-    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
-    <sheet name="config_automation_phone" r:id="rId4" sheetId="3"/>
-    <sheet name="config_fsa_pqt_build" r:id="rId5" sheetId="4"/>
-    <sheet name="config_fsa_track_build" r:id="rId6" sheetId="5"/>
+    <sheet name="config_local" sheetId="1" r:id="rId1"/>
+    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
+    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
+    <sheet name="config_automation_phone" sheetId="3" r:id="rId4"/>
+    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId5"/>
+    <sheet name="config_fsa_track_build" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="100">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -377,9 +382,6 @@
     <t>iPhone Developer: Rajesh Rao (76X824PR66)</t>
   </si>
   <si>
-    <t>browser</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -390,13 +392,15 @@
   </si>
   <si>
     <t>APP_BUNDLEID</t>
+  </si>
+  <si>
+    <t>android</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -463,29 +467,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -502,10 +506,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -540,7 +544,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -592,7 +596,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -703,21 +707,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -734,7 +738,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -786,56 +790,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747902-0905-9A4B-A648-FC506DD60323}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="65.83203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="52.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="115.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="84.0" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="74.33203125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="65.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="67" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="52.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="115.33203125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="49" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="84" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="74.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -852,7 +856,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -933,7 +937,7 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -950,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -1159,67 +1163,67 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="Q2" xr:uid="{65290685-B75F-2F47-A5A2-C5F98F0468A7}"/>
-    <hyperlink r:id="rId2" ref="S2" xr:uid="{A8C94B01-4AE8-4A46-A8C0-F0B6766D6C5A}"/>
-    <hyperlink r:id="rId3" ref="O2" xr:uid="{9021A63E-45E4-2247-B495-773BCC48D6BC}"/>
-    <hyperlink r:id="rId4" ref="U2" xr:uid="{111D145D-7C58-0241-B4B7-EC3C95D38325}"/>
-    <hyperlink r:id="rId5" ref="V2" xr:uid="{DA34061A-CC99-BD49-AFD7-59CA373B6607}"/>
-    <hyperlink r:id="rId6" ref="W2" xr:uid="{E3E98677-132E-E64D-A508-185D4810255C}"/>
-    <hyperlink r:id="rId7" ref="X2" xr:uid="{8DB1D18B-EA97-AA4D-9AC7-02A48CDE67A6}"/>
-    <hyperlink r:id="rId8" ref="Y2" xr:uid="{64F0B1C6-CD58-A845-A599-DFE23DA422CC}"/>
-    <hyperlink r:id="rId9" ref="Z2" xr:uid="{4FAFCCA4-4F24-0B49-934E-AC441897C9C5}"/>
-    <hyperlink r:id="rId10" ref="AC2" xr:uid="{486C7ACD-3F79-B144-8138-AEDF137735C6}"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="S2" r:id="rId2"/>
+    <hyperlink ref="O2" r:id="rId3"/>
+    <hyperlink ref="U2" r:id="rId4"/>
+    <hyperlink ref="V2" r:id="rId5"/>
+    <hyperlink ref="W2" r:id="rId6"/>
+    <hyperlink ref="X2" r:id="rId7"/>
+    <hyperlink ref="Y2" r:id="rId8"/>
+    <hyperlink ref="Z2" r:id="rId9"/>
+    <hyperlink ref="AC2" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BF172F-CE08-6840-ACF9-880AB6E40DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="62.1640625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1240,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -1320,9 +1324,9 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>92</v>
@@ -1337,7 +1341,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -1423,21 +1427,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{2373DCCF-7CF7-6D48-9391-B2017EA3F6CB}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{45EF8F3D-534D-2F45-94E3-C73D8504CC2F}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{317C8481-D29E-9841-A568-E5293BF078E6}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{2250E180-CC76-0844-A14E-BECC396552E1}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{3B6377D4-E37D-8E4E-A566-7D3CA80B53F6}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{08609375-5C82-1140-80FE-D1DE3470E1BE}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{195848E9-E895-054F-8CD9-4B349763F02C}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA13EFD-5466-DB43-9A70-FA51FEB925E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1446,39 +1450,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1495,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -1579,7 +1583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1587,16 +1591,16 @@
         <v>92</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -1682,61 +1686,61 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{62E806D6-9394-5B45-A604-655BD30F27F3}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{2E4CDE15-9B66-2245-B748-BCAAA05AC9E4}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{36A593B9-9976-C14C-B755-CA938AC79725}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{C4819D61-6734-1A4F-84FA-001DDBD1671D}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{A6B99C3B-70C7-E44A-A7A3-744369CCB48E}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{866CFB73-1B1F-9648-AF62-BBB387DC1218}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABD5772-2955-6C46-88A2-787F9D38DC97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +1757,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -1837,15 +1841,15 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>61</v>
@@ -1854,7 +1858,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -1940,61 +1944,61 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{FF8A98B7-8501-6F47-A2FB-10824115B353}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{E5504FE2-E34C-AD4E-9FED-91F77342117E}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{E3CFACEB-C525-FB4B-816E-5C98177D7B3A}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{037F7191-EF8F-1B41-A957-BC232B559744}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{C6F51406-8912-3748-8B88-9B0A0A8B059D}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{CDB08067-96F2-2742-872D-1B028C2950EE}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACBC21-67F9-9748-8578-54FDD50767ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -2095,9 +2099,9 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>92</v>
@@ -2106,13 +2110,13 @@
         <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -2198,20 +2202,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{A71DD4B7-4F78-624F-8526-BC2C8DAF91F2}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{1B540CF2-7A50-6B48-8B71-0C274B92DD51}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{91AEDBB0-8784-C240-9F57-F0191D9A7F37}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{4CBB3277-EAC2-1C4C-B5B0-6055F81AEB79}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{43033950-1900-2048-9098-30C4C6B77A36}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{AF882D86-8162-1A40-9D4C-2B7AFACABB92}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{F85A03DD-44E5-6E49-B503-8C6C4E7ECC22}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70778CC3-4254-DD46-A825-6190F74A8C8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -2220,40 +2224,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.1640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2270,7 +2274,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -2354,7 +2358,7 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2371,7 +2375,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>50</v>
@@ -2457,14 +2461,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{B41713CD-0C7A-A94A-9E0C-2C92C9129EB5}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{F8ED6A05-BFC1-7E48-A376-F7EF824AE76F}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{B2E95E89-7408-7140-82FB-6817D1D4C34A}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{7BA77DFF-CF38-3F44-95C3-4775F3663E98}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{A95FE44D-A1CF-E248-A845-0A3B8C68FB3D}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{DCB51B4E-919D-6847-9170-E731E9B9D69D}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{2489425F-B372-874E-8A85-A3A1E07348EE}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes for Ph_Sanity5_DVR_Mapping_Qualification_Criteria
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28315"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1"/>
+    <workbookView activeTab="3" windowHeight="16240" windowWidth="28040" xWindow="20" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" sheetId="1" r:id="rId1"/>
-    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
-    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
-    <sheet name="config_automation_phone" sheetId="3" r:id="rId4"/>
-    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId5"/>
-    <sheet name="config_fsa_track_build" sheetId="5" r:id="rId6"/>
+    <sheet name="config_local" r:id="rId1" sheetId="1"/>
+    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
+    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
+    <sheet name="config_automation_phone" r:id="rId4" sheetId="3"/>
+    <sheet name="config_fsa_pqt_build" r:id="rId5" sheetId="4"/>
+    <sheet name="config_fsa_track_build" r:id="rId6" sheetId="5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="100">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -382,10 +382,10 @@
     <t>iPhone Developer: Rajesh Rao (76X824PR66)</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>9</t>
-  </si>
-  <si>
-    <t>fsaTabletGo</t>
   </si>
   <si>
     <t>com.servicemaxinc.svmxfieldserviceapp</t>
@@ -401,6 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -467,29 +468,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -506,10 +507,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -544,7 +545,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -596,7 +597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -707,21 +708,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -738,7 +739,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -790,56 +791,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="65.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="67" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="52.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="115.33203125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="49" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="115.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="74.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="65.83203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="84.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="115.33203125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="74.33203125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -937,9 +938,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>92</v>
@@ -1163,23 +1164,542 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
-    <hyperlink ref="S2" r:id="rId2"/>
-    <hyperlink ref="O2" r:id="rId3"/>
-    <hyperlink ref="U2" r:id="rId4"/>
-    <hyperlink ref="V2" r:id="rId5"/>
-    <hyperlink ref="W2" r:id="rId6"/>
-    <hyperlink ref="X2" r:id="rId7"/>
-    <hyperlink ref="Y2" r:id="rId8"/>
-    <hyperlink ref="Z2" r:id="rId9"/>
-    <hyperlink ref="AC2" r:id="rId10"/>
+    <hyperlink r:id="rId1" ref="Q2"/>
+    <hyperlink r:id="rId2" ref="S2"/>
+    <hyperlink r:id="rId3" ref="O2"/>
+    <hyperlink r:id="rId4" ref="U2"/>
+    <hyperlink r:id="rId5" ref="V2"/>
+    <hyperlink r:id="rId6" ref="W2"/>
+    <hyperlink r:id="rId7" ref="X2"/>
+    <hyperlink r:id="rId8" ref="Y2"/>
+    <hyperlink r:id="rId9" ref="Z2"/>
+    <hyperlink r:id="rId10" ref="AC2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1188,42 +1708,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1303,13 +1821,13 @@
         <v>20</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>56</v>
@@ -1324,21 +1842,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>97</v>
@@ -1350,15 +1868,15 @@
         <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -1403,14 +1921,14 @@
       <c r="Z2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AC2" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>0</v>
@@ -1427,62 +1945,61 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1505,25 +2022,25 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>32</v>
@@ -1562,13 +2079,13 @@
         <v>20</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>56</v>
@@ -1583,7 +2100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1591,13 +2108,13 @@
         <v>92</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>96</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>97</v>
@@ -1606,79 +2123,79 @@
         <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>54</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>58</v>
+      <c r="S2" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>54</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Y2" s="7" t="s">
         <v>72</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
@@ -1686,61 +2203,62 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.1640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1763,25 +2281,25 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>32</v>
@@ -1820,13 +2338,13 @@
         <v>20</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>56</v>
@@ -1841,7 +2359,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>99</v>
       </c>
@@ -1852,10 +2370,10 @@
         <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>97</v>
@@ -1864,79 +2382,79 @@
         <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>54</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>58</v>
+      <c r="S2" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>54</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Y2" s="7" t="s">
         <v>72</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
@@ -1944,531 +2462,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added changes for config_properties.xlsx
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28315"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="16240" windowWidth="28040" xWindow="20" yWindow="460"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" r:id="rId1" sheetId="1"/>
-    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
-    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
-    <sheet name="config_automation_phone_go" r:id="rId4" sheetId="7"/>
-    <sheet name="config_automation_phone" r:id="rId5" sheetId="3"/>
-    <sheet name="config_fsa_pqt_build" r:id="rId6" sheetId="4"/>
-    <sheet name="config_fsa_track_build" r:id="rId7" sheetId="5"/>
+    <sheet name="config_local" sheetId="1" r:id="rId1"/>
+    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
+    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
+    <sheet name="config_automation_phone_go" sheetId="7" r:id="rId4"/>
+    <sheet name="config_automation_phone" sheetId="3" r:id="rId5"/>
+    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId6"/>
+    <sheet name="config_fsa_track_build" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="121">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -467,9 +467,6 @@
     <t>cs77</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>autoadmin@automation.com</t>
   </si>
   <si>
@@ -480,7 +477,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -582,34 +578,34 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -626,10 +622,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -664,7 +660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -716,7 +712,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -827,21 +823,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -858,7 +854,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -910,61 +906,61 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="98.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="49.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.1640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="48.83203125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="43.83203125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.83203125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="98.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="49.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="48.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1070,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -1082,7 +1078,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -1121,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>17</v>
@@ -1130,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>52</v>
@@ -1273,21 +1269,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" r:id="rId2" ref="W2"/>
-    <hyperlink r:id="rId3" ref="Y2"/>
-    <hyperlink r:id="rId4" ref="O2"/>
-    <hyperlink r:id="rId5" ref="Q2"/>
-    <hyperlink r:id="rId6" ref="S2"/>
-    <hyperlink r:id="rId7" ref="X2"/>
-    <hyperlink r:id="rId8" ref="Z2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="W2" r:id="rId2" display="https://cs70.salesforce.com/services/data/v42.0/query/?q="/>
+    <hyperlink ref="Y2" r:id="rId3"/>
+    <hyperlink ref="O2" r:id="rId4"/>
+    <hyperlink ref="Q2" r:id="rId5"/>
+    <hyperlink ref="S2" r:id="rId6"/>
+    <hyperlink ref="X2" r:id="rId7"/>
+    <hyperlink ref="Z2" r:id="rId8"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="AD1" workbookViewId="0">
@@ -1296,43 +1292,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="31" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="62.1640625" customWidth="1" collapsed="1"/>
+    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1442,7 +1438,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1554,21 +1550,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
-    <hyperlink r:id="rId7" ref="AC2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
@@ -1577,41 +1573,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1721,7 +1717,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -1833,19 +1829,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
@@ -1854,40 +1850,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="93.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="31" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2111,56 +2107,56 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2270,7 +2266,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -2278,7 +2274,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -2382,19 +2378,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -2403,42 +2399,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2548,7 +2544,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2660,20 +2656,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
-    <hyperlink r:id="rId7" ref="AC2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="AE1" workbookViewId="0">
@@ -2682,42 +2678,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.83203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.1640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2827,7 +2823,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -2939,14 +2935,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2"/>
-    <hyperlink r:id="rId2" ref="V2"/>
-    <hyperlink r:id="rId3" ref="W2"/>
-    <hyperlink r:id="rId4" ref="X2"/>
-    <hyperlink r:id="rId5" ref="Y2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
-    <hyperlink r:id="rId7" ref="AC2"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="X2" r:id="rId4"/>
+    <hyperlink ref="Y2" r:id="rId5"/>
+    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink ref="AC2" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing changes made to 10563
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="16620" windowWidth="28800" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" sheetId="1" r:id="rId1"/>
-    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
-    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
-    <sheet name="config_automation_phone_go" sheetId="7" r:id="rId4"/>
-    <sheet name="config_automation_phone" sheetId="3" r:id="rId5"/>
-    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId6"/>
-    <sheet name="config_fsa_track_build" sheetId="8" r:id="rId7"/>
+    <sheet name="config_local" r:id="rId1" sheetId="1"/>
+    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
+    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
+    <sheet name="config_automation_phone_go" r:id="rId4" sheetId="7"/>
+    <sheet name="config_automation_phone" r:id="rId5" sheetId="3"/>
+    <sheet name="config_fsa_pqt_build" r:id="rId6" sheetId="4"/>
+    <sheet name="config_fsa_track_build" r:id="rId7" sheetId="8"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="143">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -523,11 +523,15 @@
   <si>
     <t>a2D0U000000DTf6UAG</t>
   </si>
+  <si>
+    <t>false</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -622,35 +626,35 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -667,10 +671,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -705,7 +709,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -757,7 +761,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -868,21 +872,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -899,7 +903,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -951,14 +955,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -967,45 +971,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="98.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="49.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="48.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="98.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="49.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="48.83203125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="43.83203125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.83203125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1115,7 +1119,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -1314,21 +1318,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="W2" r:id="rId2" display="https://cs70.salesforce.com/services/data/v42.0/query/?q="/>
-    <hyperlink ref="Y2" r:id="rId3"/>
-    <hyperlink ref="O2" r:id="rId4"/>
-    <hyperlink ref="Q2" r:id="rId5"/>
-    <hyperlink ref="S2" r:id="rId6"/>
-    <hyperlink ref="X2" r:id="rId7"/>
-    <hyperlink ref="Z2" r:id="rId8"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" r:id="rId2" ref="W2"/>
+    <hyperlink r:id="rId3" ref="Y2"/>
+    <hyperlink r:id="rId4" ref="O2"/>
+    <hyperlink r:id="rId5" ref="Q2"/>
+    <hyperlink r:id="rId6" ref="S2"/>
+    <hyperlink r:id="rId7" ref="X2"/>
+    <hyperlink r:id="rId8" ref="Z2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
@@ -1337,43 +1341,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="31" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1595,21 +1599,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1618,41 +1622,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1762,7 +1766,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -1874,19 +1878,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -1895,41 +1899,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="93.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2154,14 +2158,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="Q2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2170,43 +2174,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="30" max="31" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2316,7 +2320,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2428,19 +2432,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2449,42 +2453,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2706,20 +2710,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2728,7 +2732,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2953,17 +2957,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="X2" r:id="rId4"/>
-    <hyperlink ref="Y2" r:id="rId5"/>
-    <hyperlink ref="Z2" r:id="rId6"/>
-    <hyperlink ref="AC2" r:id="rId7"/>
-    <hyperlink ref="O2" r:id="rId8"/>
-    <hyperlink ref="Q2" r:id="rId9"/>
-    <hyperlink ref="S2" r:id="rId10"/>
+    <hyperlink r:id="rId1" ref="U2"/>
+    <hyperlink r:id="rId2" ref="V2"/>
+    <hyperlink r:id="rId3" ref="W2"/>
+    <hyperlink r:id="rId4" ref="X2"/>
+    <hyperlink r:id="rId5" ref="Y2"/>
+    <hyperlink r:id="rId6" ref="Z2"/>
+    <hyperlink r:id="rId7" ref="AC2"/>
+    <hyperlink r:id="rId8" ref="O2"/>
+    <hyperlink r:id="rId9" ref="Q2"/>
+    <hyperlink r:id="rId10" ref="S2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new fixes for sahi execution
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76AE15F-8769-2947-BE90-882F1B338105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{4C1BB827-F794-914C-92D4-F10662A052F3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="16620" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" sheetId="1" r:id="rId1"/>
-    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
-    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
-    <sheet name="config_automation_phone_go" sheetId="7" r:id="rId4"/>
-    <sheet name="config_automation_phone" sheetId="3" r:id="rId5"/>
-    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId6"/>
-    <sheet name="config_fsa_track_build" sheetId="8" r:id="rId7"/>
+    <sheet name="config_local" r:id="rId1" sheetId="1"/>
+    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
+    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
+    <sheet name="config_automation_phone_go" r:id="rId4" sheetId="7"/>
+    <sheet name="config_automation_phone" r:id="rId5" sheetId="3"/>
+    <sheet name="config_fsa_pqt_build" r:id="rId6" sheetId="4"/>
+    <sheet name="config_fsa_track_build" r:id="rId7" sheetId="8"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="143">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -524,11 +524,15 @@
   <si>
     <t>a2D0U000000DTf6UAG</t>
   </si>
+  <si>
+    <t>false</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -623,35 +627,35 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -668,10 +672,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -706,7 +710,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -758,7 +762,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -869,21 +873,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -900,7 +904,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -952,14 +956,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -968,45 +972,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="54" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="98.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="49.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="48.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="98.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="49.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="48.83203125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="43.83203125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.83203125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1116,7 +1120,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -1315,66 +1319,66 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="W2" r:id="rId2" display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="Y2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="O2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="Q2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="S2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="X2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="Z2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" r:id="rId2" ref="W2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId3" ref="Y2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink r:id="rId4" ref="O2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Q2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink r:id="rId6" ref="S2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink r:id="rId7" ref="X2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink r:id="rId8" ref="Z2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="31" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1596,21 +1600,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1619,41 +1623,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -1875,19 +1879,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -1896,41 +1900,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="93.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2155,14 +2159,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink r:id="rId1" ref="Q2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2171,43 +2175,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="30" max="31" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2317,7 +2321,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2429,19 +2433,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2450,42 +2454,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2595,7 +2599,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2707,29 +2711,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="27.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2954,17 +2959,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="O2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="Q2" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="S2" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink r:id="rId8" ref="O2" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink r:id="rId9" ref="Q2" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink r:id="rId10" ref="S2" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding salesforceID to config sheet
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1917,8 +1917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1952,7 +1952,7 @@
     <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="22.83203125" customWidth="1" collapsed="1"/>
     <col min="32" max="33" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="34" max="34" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
Changed Platform name to ios for config_Automation_Build
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{604AB9B0-23E8-234B-AFBE-7D15E232F3B2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1D03534-18BD-6F46-AD76-6CCDBCABF613}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="16460" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="config_local" r:id="rId1" sheetId="1"/>
-    <sheet name="config_automation_build" r:id="rId2" sheetId="2"/>
-    <sheet name="config_automation_tablet_go" r:id="rId3" sheetId="6"/>
-    <sheet name="config_automation_phone_go" r:id="rId4" sheetId="7"/>
-    <sheet name="config_automation_phone" r:id="rId5" sheetId="3"/>
-    <sheet name="config_fsa_pqt_build" r:id="rId6" sheetId="4"/>
-    <sheet name="config_fsa_track_build" r:id="rId7" sheetId="8"/>
+    <sheet name="config_local" sheetId="1" r:id="rId1"/>
+    <sheet name="config_automation_build" sheetId="2" r:id="rId2"/>
+    <sheet name="config_automation_tablet_go" sheetId="6" r:id="rId3"/>
+    <sheet name="config_automation_phone_go" sheetId="7" r:id="rId4"/>
+    <sheet name="config_automation_phone" sheetId="3" r:id="rId5"/>
+    <sheet name="config_fsa_pqt_build" sheetId="4" r:id="rId6"/>
+    <sheet name="config_fsa_track_build" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="143">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -544,7 +544,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -646,35 +645,35 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="12" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -691,10 +690,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -729,7 +728,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -781,7 +780,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -892,21 +891,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -923,7 +922,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -975,14 +974,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
@@ -991,45 +990,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="98.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="49.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.1640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="48.83203125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="43.83203125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.83203125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="98.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="49.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="48.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -1338,66 +1337,66 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" r:id="rId2" ref="W2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink r:id="rId3" ref="Y2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink r:id="rId4" ref="O2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Q2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink r:id="rId6" ref="S2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink r:id="rId7" ref="X2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink r:id="rId8" ref="Z2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="W2" r:id="rId2" display="https://cs70.salesforce.com/services/data/v42.0/query/?q=" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="Y2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="S2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="X2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="Z2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="40.5" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="40.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="62.1640625" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1510,9 +1509,9 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>89</v>
@@ -1625,21 +1624,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1648,41 +1647,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1904,61 +1903,61 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="53.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="74.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="50.5" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="45.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="93.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="77.83203125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="31" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="74.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="50.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -2182,12 +2181,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
@@ -2196,45 +2195,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="34.33203125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="22.83203125" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2462,19 +2461,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2483,42 +2482,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.5" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="51.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="99.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="71.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="103.1640625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="62.1640625" collapsed="true"/>
-    <col min="30" max="32" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="24.83203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="51.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="99.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="71.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="70.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="103.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="62.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2740,20 +2739,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2984,17 +2983,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink r:id="rId2" ref="V2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink r:id="rId3" ref="W2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink r:id="rId4" ref="X2" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink r:id="rId5" ref="Y2" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink r:id="rId6" ref="Z2" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink r:id="rId7" ref="AC2" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink r:id="rId8" ref="O2" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink r:id="rId9" ref="Q2" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink r:id="rId10" ref="S2" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="W2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="X2" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="Z2" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="AC2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="O2" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="Q2" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="S2" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes for technician1 user
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/config_properties.xlsx
+++ b/fsaautomation/resources/config_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1D03534-18BD-6F46-AD76-6CCDBCABF613}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B387DA-0C1B-D94D-95C1-12E293F47C99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config_local" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="143">
   <si>
     <t>0053D000001fEk6QAE</t>
   </si>
@@ -384,30 +384,12 @@
     <t>android</t>
   </si>
   <si>
-    <t>8.1.0</t>
-  </si>
-  <si>
     <t>technician@qa.com</t>
   </si>
   <si>
     <t>servicemax19</t>
   </si>
   <si>
-    <r>
-      <t>auto-tech1</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF4180FF"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>@svmx.com</t>
-    </r>
-  </si>
-  <si>
     <t>automation@qa.com</t>
   </si>
   <si>
@@ -538,13 +520,19 @@
   </si>
   <si>
     <t>a2D0U000000DTf6UAG</t>
+  </si>
+  <si>
+    <t>0050U000001VyhCQAS</t>
+  </si>
+  <si>
+    <t>technician1@qa.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -600,13 +588,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF4180FF"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3933FF"/>
       <name val="Monaco"/>
@@ -647,7 +628,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -664,7 +645,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -982,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ31"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,13 +1110,13 @@
         <v>36</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1146,13 +1127,13 @@
         <v>89</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>92</v>
@@ -1185,7 +1166,7 @@
         <v>30</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>16</v>
@@ -1194,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>51</v>
@@ -1239,101 +1220,14 @@
         <v>37</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I31" s="2"/>
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1354,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1382,7 @@
         <v>53</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF1" s="3" t="s">
         <v>39</v>
@@ -1500,13 +1394,13 @@
         <v>36</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AK1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1411,7 @@
         <v>89</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -1598,7 +1492,7 @@
         <v>77</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AE2" s="5" t="s">
         <v>0</v>
@@ -1613,13 +1507,13 @@
         <v>37</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1782,13 +1676,13 @@
         <v>36</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1799,13 +1693,13 @@
         <v>89</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>92</v>
@@ -1892,13 +1786,13 @@
         <v>37</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1916,10 +1810,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1953,14 +1847,15 @@
     <col min="27" max="27" width="45.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="93.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="77.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="32" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="23.33203125" customWidth="1"/>
+    <col min="31" max="31" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="24.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="28.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2052,25 +1947,28 @@
         <v>53</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" s="14" t="s">
-        <v>113</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>94</v>
       </c>
@@ -2078,13 +1976,13 @@
         <v>12.1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>92</v>
@@ -2114,73 +2012,79 @@
         <v>44</v>
       </c>
       <c r="O2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="T2" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U2" s="13" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="Y2" s="13" t="s">
         <v>69</v>
       </c>
       <c r="Z2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AD2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AE2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="AD2" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AG2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AF2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ2" s="14" t="s">
-        <v>116</v>
+      <c r="AK2" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{A172A620-4AD2-0241-A833-4897AD42C8E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2325,7 +2229,7 @@
         <v>53</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF1" s="3" t="s">
         <v>39</v>
@@ -2337,13 +2241,13 @@
         <v>36</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AK1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2354,13 +2258,13 @@
         <v>89</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>92</v>
@@ -2435,7 +2339,7 @@
         <v>84</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AE2" s="5" t="s">
         <v>0</v>
@@ -2450,13 +2354,13 @@
         <v>37</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2618,13 +2522,13 @@
         <v>36</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2728,13 +2632,13 @@
         <v>37</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="AJ2" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2862,13 +2766,13 @@
         <v>36</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -2885,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>92</v>
@@ -2915,70 +2819,70 @@
         <v>44</v>
       </c>
       <c r="O2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="X2" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="Y2" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Z2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AC2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="AB2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AD2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>